<commit_message>
modifed mosavi is added
</commit_message>
<xml_diff>
--- a/insurance.xlsx
+++ b/insurance.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="217">
   <si>
     <t xml:space="preserve">هادی خانیا </t>
   </si>
@@ -679,6 +679,15 @@
   </si>
   <si>
     <t>اقای داوریان سامان</t>
+  </si>
+  <si>
+    <t>علي اصغر پورموسوي</t>
+  </si>
+  <si>
+    <t>ثالث -تیبا</t>
+  </si>
+  <si>
+    <t>1402/10/10</t>
   </si>
 </sst>
 </file>
@@ -1483,8 +1492,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:LN106"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="B58" workbookViewId="0">
+      <selection activeCell="G68" sqref="G68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25"/>
@@ -5011,18 +5020,26 @@
       <c r="A68" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="B68" s="19"/>
+      <c r="B68" s="19" t="s">
+        <v>214</v>
+      </c>
       <c r="C68" s="34" t="s">
-        <v>90</v>
-      </c>
-      <c r="D68" s="19"/>
-      <c r="E68" s="19"/>
-      <c r="F68" s="5"/>
+        <v>216</v>
+      </c>
+      <c r="D68" s="19">
+        <v>6842785</v>
+      </c>
+      <c r="E68" s="19" t="s">
+        <v>215</v>
+      </c>
+      <c r="F68" s="5">
+        <v>28262236</v>
+      </c>
       <c r="G68" s="6"/>
       <c r="H68" s="5"/>
       <c r="I68" s="7">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>28262236</v>
       </c>
       <c r="J68" s="16"/>
       <c r="K68" s="17"/>

</xml_diff>